<commit_message>
Fresh org data changes
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/credentials.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/credentials.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>UserName</t>
   </si>
@@ -45,13 +45,28 @@
   </si>
   <si>
     <t>servicemax12</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>005q0000003RLoJ</t>
+  </si>
+  <si>
+    <t>commonuser@sf1.com.full1</t>
+  </si>
+  <si>
+    <t>servicemax1</t>
+  </si>
+  <si>
+    <t>0051g000000NHRb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -84,6 +99,21 @@
       <sz val="11"/>
       <color rgb="FF3933FF"/>
       <name val="Monaco"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,7 +133,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="28">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -132,8 +162,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -148,8 +180,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="28">
+  <cellStyles count="30">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -164,6 +198,8 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -452,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,6 +517,9 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -492,8 +531,24 @@
       <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>